<commit_message>
Build REST API in index.js with Express
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -12,7 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="5784"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Documentation" sheetId="1" r:id="rId1"/>
+    <sheet name="For html" sheetId="3" r:id="rId2"/>
+    <sheet name="tables" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="59">
   <si>
     <t>Return a list of ALL movies to the user;</t>
   </si>
@@ -87,9 +89,6 @@
   </si>
   <si>
     <t>birthday</t>
-  </si>
-  <si>
-    <t>rip</t>
   </si>
   <si>
     <t>bio</t>
@@ -211,6 +210,15 @@
 birthyear:
 deathyear:
 }</t>
+  </si>
+  <si>
+    <t>deathdate</t>
+  </si>
+  <si>
+    <t>JSON object holding data about the movie that was added, including an ID:</t>
+  </si>
+  <si>
+    <t>A JSON object holding data about the director that was added, including an ID</t>
   </si>
 </sst>
 </file>
@@ -316,7 +324,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -329,6 +337,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -611,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,7 +633,7 @@
     <col min="3" max="3" width="21.21875" customWidth="1"/>
     <col min="4" max="4" width="16.44140625" customWidth="1"/>
     <col min="5" max="6" width="79.44140625" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="7" max="7" width="68.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -638,10 +647,10 @@
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -649,16 +658,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="144" x14ac:dyDescent="0.3">
@@ -666,16 +675,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -689,10 +698,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
@@ -700,7 +709,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -709,7 +718,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -717,16 +726,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -734,16 +743,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -751,16 +760,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -768,16 +777,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -785,16 +794,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -804,98 +813,315 @@
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G19" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="68.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="4" t="s">
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="F4" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="7"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="8"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="8"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="7"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="7"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="4" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>